<commit_message>
Adição de novos arquivos
</commit_message>
<xml_diff>
--- a/lojistas.xlsx
+++ b/lojistas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\boletinho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AD72F0-3DF6-4EEE-8413-A0755EB40D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D7573B-CBA3-48B8-AA47-FAB288F6B718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{317DF3BE-0FEE-454E-8665-C5BEFCB5FC54}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11385" xr2:uid="{317DF3BE-0FEE-454E-8665-C5BEFCB5FC54}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Controle</t>
   </si>
   <si>
-    <t>OEK0626</t>
-  </si>
-  <si>
     <t>Cnpj</t>
   </si>
   <si>
@@ -50,13 +47,13 @@
     <t>Placa</t>
   </si>
   <si>
-    <t>3500000</t>
-  </si>
-  <si>
-    <t>4100000</t>
-  </si>
-  <si>
     <t>01.569.286/0001-93</t>
+  </si>
+  <si>
+    <t>OEK0628</t>
+  </si>
+  <si>
+    <t>4575000</t>
   </si>
 </sst>
 </file>
@@ -108,12 +105,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +428,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,59 +436,47 @@
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="C4" s="1"/>
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>